<commit_message>
CurrentDraw: Tweak Table Headings
</commit_message>
<xml_diff>
--- a/2016-11-23 Teensy 3.6 Current Draw/2016-11-14 Teensy 3.6 Current Draw for Blog.xlsx
+++ b/2016-11-23 Teensy 3.6 Current Draw/2016-11-14 Teensy 3.6 Current Draw for Blog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="11055" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="11055"/>
   </bookViews>
   <sheets>
     <sheet name="Pretty Table" sheetId="4" r:id="rId1"/>
@@ -87,11 +87,11 @@
 asm(" WFI");</t>
   </si>
   <si>
-    <t>Estimated Battery Life</t>
+    <t>Capacity
+(mA-hr)</t>
   </si>
   <si>
-    <t>Capacity
-(mA-hr)</t>
+    <t>Estimated Battery Life (Hrs)</t>
   </si>
 </sst>
 </file>
@@ -407,11 +407,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222118656"/>
-        <c:axId val="222120192"/>
+        <c:axId val="149636608"/>
+        <c:axId val="149638144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222118656"/>
+        <c:axId val="149636608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="240"/>
@@ -423,13 +423,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222120192"/>
+        <c:crossAx val="149638144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222120192"/>
+        <c:axId val="149638144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222118656"/>
+        <c:crossAx val="149636608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -724,11 +724,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222141056"/>
-        <c:axId val="222364416"/>
+        <c:axId val="149659008"/>
+        <c:axId val="149661184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222141056"/>
+        <c:axId val="149659008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -759,13 +759,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222364416"/>
+        <c:crossAx val="149661184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222364416"/>
+        <c:axId val="149661184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -796,7 +796,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222141056"/>
+        <c:crossAx val="149659008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1080,11 +1080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222386048"/>
-        <c:axId val="222392320"/>
+        <c:axId val="149582208"/>
+        <c:axId val="149584128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222386048"/>
+        <c:axId val="149582208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -1119,12 +1119,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222392320"/>
+        <c:crossAx val="149584128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222392320"/>
+        <c:axId val="149584128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1155,7 +1155,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222386048"/>
+        <c:crossAx val="149582208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1479,11 +1479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222091520"/>
-        <c:axId val="222093696"/>
+        <c:axId val="149684992"/>
+        <c:axId val="149686912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222091520"/>
+        <c:axId val="149684992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="260"/>
@@ -1514,13 +1514,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222093696"/>
+        <c:crossAx val="149686912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="60"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222093696"/>
+        <c:axId val="149686912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1550,7 +1550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222091520"/>
+        <c:crossAx val="149684992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2315,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2330,7 +2330,8 @@
     <col min="7" max="7" width="13.140625" style="7" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="6"/>
     <col min="10" max="10" width="12.42578125" style="6" customWidth="1"/>
-    <col min="11" max="12" width="16" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="16" style="6" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -2368,7 +2369,7 @@
         <v>17</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L7" s="22"/>
     </row>
@@ -2396,7 +2397,7 @@
         <v>15</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>20</v>
@@ -2760,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>

</xml_diff>